<commit_message>
Changes needed for lake profiles
</commit_message>
<xml_diff>
--- a/IR_uses_standards.xlsx
+++ b/IR_uses_standards.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" tabRatio="577" firstSheet="3" activeTab="6"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" tabRatio="577" firstSheet="3" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="PolyToTableMatch_BU" sheetId="4" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8440" uniqueCount="1032">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8470" uniqueCount="1035">
   <si>
     <t>WaterbodyTypes</t>
   </si>
@@ -3145,6 +3145,15 @@
   </si>
   <si>
     <t>Chronic ELS</t>
+  </si>
+  <si>
+    <t>Profile depth</t>
+  </si>
+  <si>
+    <t>Minimum Dissolved Oxygen</t>
+  </si>
+  <si>
+    <t>m</t>
   </si>
 </sst>
 </file>
@@ -29663,11 +29672,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K93"/>
+  <dimension ref="A1:K99"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B95" sqref="B95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32336,6 +32345,132 @@
       </c>
       <c r="K93" t="s">
         <v>1006</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>1032</v>
+      </c>
+      <c r="B94" t="s">
+        <v>10</v>
+      </c>
+      <c r="K94" t="s">
+        <v>1034</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>1032</v>
+      </c>
+      <c r="B95" t="s">
+        <v>11</v>
+      </c>
+      <c r="K95" t="s">
+        <v>1034</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B96" t="s">
+        <v>10</v>
+      </c>
+      <c r="E96" t="s">
+        <v>995</v>
+      </c>
+      <c r="F96" t="s">
+        <v>995</v>
+      </c>
+      <c r="G96">
+        <v>1</v>
+      </c>
+      <c r="H96" t="s">
+        <v>1001</v>
+      </c>
+      <c r="J96">
+        <v>5</v>
+      </c>
+      <c r="K96" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B97" t="s">
+        <v>11</v>
+      </c>
+      <c r="E97" t="s">
+        <v>995</v>
+      </c>
+      <c r="F97" t="s">
+        <v>995</v>
+      </c>
+      <c r="G97">
+        <v>1</v>
+      </c>
+      <c r="H97" t="s">
+        <v>1001</v>
+      </c>
+      <c r="J97">
+        <v>3</v>
+      </c>
+      <c r="K97" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>934</v>
+      </c>
+      <c r="B98" t="s">
+        <v>10</v>
+      </c>
+      <c r="E98" t="s">
+        <v>994</v>
+      </c>
+      <c r="F98" t="s">
+        <v>994</v>
+      </c>
+      <c r="G98">
+        <v>1</v>
+      </c>
+      <c r="H98" t="s">
+        <v>1001</v>
+      </c>
+      <c r="J98">
+        <v>20</v>
+      </c>
+      <c r="K98" t="s">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>934</v>
+      </c>
+      <c r="B99" t="s">
+        <v>11</v>
+      </c>
+      <c r="E99" t="s">
+        <v>994</v>
+      </c>
+      <c r="F99" t="s">
+        <v>994</v>
+      </c>
+      <c r="G99">
+        <v>1</v>
+      </c>
+      <c r="H99" t="s">
+        <v>1001</v>
+      </c>
+      <c r="J99">
+        <v>27</v>
+      </c>
+      <c r="K99" t="s">
+        <v>1013</v>
       </c>
     </row>
   </sheetData>
@@ -33547,7 +33682,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>